<commit_message>
Little bit of Schedule update
</commit_message>
<xml_diff>
--- a/Documentation/Schedules 2.0.xlsx
+++ b/Documentation/Schedules 2.0.xlsx
@@ -138,21 +138,21 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Work on final presentation
+    <t>Finalization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day6 Alpha </t>
+  </si>
+  <si>
+    <t>Day 8 Beta</t>
+  </si>
+  <si>
+    <t>Day 9 Finish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cover manny in his absence
 Finish unity sprite implementation for chicken run game 
 </t>
-  </si>
-  <si>
-    <t>Finalization</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Day6 Alpha </t>
-  </si>
-  <si>
-    <t>Day 8 Beta</t>
-  </si>
-  <si>
-    <t>Day 9 Finish</t>
   </si>
 </sst>
 </file>
@@ -426,30 +426,30 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="43.140625" customWidth="1"/>
-    <col min="4" max="4" width="45" customWidth="1"/>
-    <col min="6" max="6" width="46.5703125" customWidth="1"/>
+    <col min="2" max="2" width="109.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="70.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="70.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="55.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>1</v>
@@ -549,10 +549,10 @@
         <v>27</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>14</v>

</xml_diff>